<commit_message>
Added notes and calculation of log(2) to 100 digits.
</commit_message>
<xml_diff>
--- a/notes/exponents/exponents.xlsx
+++ b/notes/exponents/exponents.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gowork\src\MikeAustin71\mathopsgo\notes\exponents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B600B80-F1C7-4E2F-9722-A0A4D268F653}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E8B862-8DFC-4433-BDB1-BCB222C646E4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8595" activeTab="2" xr2:uid="{4742039C-2FA1-473E-BACF-12A29DC1045D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8595" activeTab="1" xr2:uid="{4742039C-2FA1-473E-BACF-12A29DC1045D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>m</t>
   </si>
@@ -224,6 +225,9 @@
   </si>
   <si>
     <t>n=</t>
+  </si>
+  <si>
+    <t>2^3.5</t>
   </si>
 </sst>
 </file>
@@ -1330,8 +1334,8 @@
       <xdr:rowOff>94138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="397352" cy="375680"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1413,7 +1417,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1772,9 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF53373-F66D-48E4-A24A-6B7498CEACDC}">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
-    </sheetView>
+    <sheetView topLeftCell="A43" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2253,6 +2255,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829DAACF-A53F-459B-A8BD-F57FFCED6718}">
+  <dimension ref="C3:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3">
+        <f>POWER(2, 3.5)</f>
+        <v>11.313708498984759</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f xml:space="preserve"> C5*E5*G5</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f>5^0.5</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f>+E3-H5</f>
+        <v>3.3137084989847594</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B79DAFD-F4E5-4ADD-BA9F-08C03119CF52}">
   <dimension ref="B5:S21"/>
   <sheetViews>
@@ -2406,11 +2473,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CA25F7-72DE-439B-BF2A-31649685D937}">
   <dimension ref="A2:K192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>